<commit_message>
List of all current and planned recipes
Initial Commit
</commit_message>
<xml_diff>
--- a/20170817_Grasshopper_Recipe_List.xlsx
+++ b/20170817_Grasshopper_Recipe_List.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cjp.co.uk\London\Genesys\08_Research\01_Working_Groups\01_Building_Physics\Standardisation\Grasshopper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cjp.co.uk\London\Genesys\10_Software\Rhinoceros\Grasshopper Recipes\For Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9828" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard_Simulations" sheetId="1" r:id="rId1"/>
     <sheet name="Experimental_Simulations" sheetId="2" r:id="rId2"/>
+    <sheet name="Dynamo_Simulations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -189,8 +190,90 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Wealend, Edwin</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{302E939E-6369-4002-96CB-B84E75EC13EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wealend, Edwin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Initials of the original creator or editor of the recipe. If significantly revised/forked, should be the initials of the reviser.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{554BFC82-ACC7-456E-8634-C970936B9153}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wealend, Edwin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Initials of checker. Checker should be a competent and regular Grasshopper user. If in doubt about competence of local staff to check, ask EW.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{A947D31C-00A5-4CCC-92D7-566BE67A04F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Wealend, Edwin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Initials of verifier. Should be a Principal Engineer or higher, competent in the category of simulation and able to compare against experience and rules of thumb.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="99">
   <si>
     <t>Daylight</t>
   </si>
@@ -463,6 +546,30 @@
   </si>
   <si>
     <t>EXP</t>
+  </si>
+  <si>
+    <t>ROOMS_TO_SPACES</t>
+  </si>
+  <si>
+    <t>Creates analytical spaces from rooms and imports relevant details for analysis.</t>
+  </si>
+  <si>
+    <t>SPACE_SCHEDULE</t>
+  </si>
+  <si>
+    <t>Creates a space schedule to allow interrogation of validity</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Standard DF calculation with CIE overcast sky and Energy Plus simple energy calculation from simple DWG file. Takes one set of window curves and internal wall curves</t>
+  </si>
+  <si>
+    <t>DF_ENE</t>
+  </si>
+  <si>
+    <t>AR</t>
   </si>
 </sst>
 </file>
@@ -510,7 +617,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -617,11 +730,78 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1202,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1395,7 @@
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="120.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="120.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="9.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" style="1" customWidth="1"/>
@@ -1355,7 +1535,7 @@
         <v>82</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>68</v>
@@ -1388,7 +1568,7 @@
         <v>83</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>68</v>
@@ -1463,17 +1643,17 @@
         <v>45</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f t="shared" ref="F9:F32" si="1">_xlfn.TEXTJOIN("_",TRUE, A9,B9,C9,D9,E9)</f>
+        <f t="shared" ref="F9:F31" si="1">_xlfn.TEXTJOIN("_",TRUE, A9,B9,C9,D9,E9)</f>
         <v>BP_DL_02_001_CBDM_sDA_ASE</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1526,14 +1706,14 @@
         <v>56</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_DL_04_001_CBDM_DA</v>
+        <v>BP_DL_04_001_LEED_DF</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>76</v>
@@ -1557,71 +1737,73 @@
         <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_DL_05_001_LEED_DF</v>
+        <v>BP_DL_05_001_CBDM_MELLUX</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="4" t="str">
+      <c r="A13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_DL_06_001_CBDM_MELLUX</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="3" t="s">
+        <v>BP_PLN_01_001_ROL</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1631,27 +1813,25 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_PLN_01_001_ROL</v>
+        <v>BP_PLN_02_001_SOL_ENVELOPE</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1664,77 +1844,79 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>BP_PLN_02_001_SOL_ENVELOPE</v>
+        <f t="shared" ref="F16" si="2">_xlfn.TEXTJOIN("_",TRUE, A16,B16,C16,D16,E16)</f>
+        <v>BP_PLN_03_001_SOL_RADIATION</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="4" t="str">
-        <f t="shared" ref="F17" si="2">_xlfn.TEXTJOIN("_",TRUE, A17,B17,C17,D17,E17)</f>
-        <v>BP_PLN_03_001_SOL_RADIATION</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_01_001_PMV_PPD</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1744,27 +1926,25 @@
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_01_001_PMV_PPD</v>
+        <v>BP_TC_02_001_ASHRAE_ADAPTIVE</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1777,20 +1957,20 @@
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_02_001_ASHRAE_ADAPTIVE</v>
+        <v>BP_TC_03_001_CIBSE_ADAPTIVE</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>76</v>
@@ -1808,25 +1988,27 @@
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_03_001_CIBSE_ADAPTIVE</v>
+        <v>BP_TC_04_001_TC_MAPPING</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1839,27 +2021,25 @@
         <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_04_001_TC_MAPPING</v>
+        <v>BP_TC_05_001_EXT_LAWSONS</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1872,77 +2052,79 @@
         <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_05_001_EXT_LAWSONS</v>
+        <v>BP_TC_06_001_EXT_UTCI</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="4" t="str">
+      <c r="A24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_TC_06_001_EXT_UTCI</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="9"/>
+        <v>BP_GLR_01_001_GLARE</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -1952,77 +2134,75 @@
         <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_GLR_01_001_GLARE</v>
+        <v>BP_GLR_02_001_DGP</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="4" t="str">
+      <c r="A27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_GLR_02_001_DGP</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="3" t="s">
+        <v>BP_LOAD_01_001_CIBSE_LOAD</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="9"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -2032,20 +2212,20 @@
         <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>BP_LOAD_01_001_CIBSE_LOAD</v>
+        <v>BP_LOAD_02_001_ASHRAE_LOAD</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>76</v>
@@ -2056,115 +2236,84 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>BP_LOAD_02_001_ASHRAE_LOAD</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="A30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="A31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="F31" s="4" t="str">
         <f t="shared" si="1"/>
         <v>BP_ENE_01_001_IDEAL_SYSTEM</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H3:H6 H8:H13 H15:H16 H19:H24 H26:H27 H29:H30 H32">
-    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="ALMOST">
+  <conditionalFormatting sqref="H3:H6 H14:H15 H18:H23 H25:H26 H28:H29 H31 H8:H12">
+    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="14" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H6">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="ALMOST">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="25" priority="8" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="24" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="ALMOST">
-      <formula>NOT(ISERROR(SEARCH("ALMOST",H17)))</formula>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="ALMOST">
+      <formula>NOT(ISERROR(SEARCH("ALMOST",H16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",H17)))</formula>
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",H16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",H17)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",H16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2177,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2188,7 +2337,7 @@
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="120.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="133" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="9.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" style="1" customWidth="1"/>
@@ -2281,14 +2430,31 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE, A4,B4,C4,D4,E4)</f>
+        <v>BP_EXP_01_001_DF_ENE</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -2702,46 +2868,983 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="ALMOST">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H6 H8:H13 H15:H16 H20:H25 H27:H28 H30:H31 H33">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="ALMOST">
+  <conditionalFormatting sqref="H8:H13 H15:H16 H20:H25 H27:H28 H30:H31 H33 H3:H6">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H6">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="ALMOST">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="ALMOST">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="ALMOST">
       <formula>NOT(ISERROR(SEARCH("ALMOST",H17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",H17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",H17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A644A6BE-9BA7-4FB1-A4E1-388EA4A92D01}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE, A3,B3,C3,D3,E3)</f>
+        <v>BP_GEN_00_001_DEFAULT</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f t="shared" ref="F5:F6" si="0">_xlfn.TEXTJOIN("_",TRUE, A5,B5,C5,D5,E5)</f>
+        <v>BP_GEO_01_001_ROOMS_TO_SPACES</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>BP_GEO_02_001_SPACE_SCHEDULE</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="18" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE, A8,B8,C8,D8,E8)</f>
+        <v>BP_DL_01_001_DF</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="12" t="str">
+        <f t="shared" ref="F9:F32" si="1">_xlfn.TEXTJOIN("_",TRUE, A9,B9,C9,D9,E9)</f>
+        <v>BP_DL_02_001_CBDM_sDA_ASE</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_DL_03_001_CBDM_UDI</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_DL_04_001_CBDM_DA</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_DL_05_001_LEED_DF</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_DL_06_001_CBDM_MELLUX</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_PLN_01_001_ROL</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_PLN_02_001_SOL_ENVELOPE</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_PLN_03_001_SOL_RADIATION</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_01_001_PMV_PPD</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_02_001_ASHRAE_ADAPTIVE</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_03_001_CIBSE_ADAPTIVE</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_04_001_TC_MAPPING</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_05_001_EXT_LAWSONS</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_TC_06_001_EXT_UTCI</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_GLR_01_001_GLARE</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_GLR_02_001_DGP</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:12" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
+    </row>
+    <row r="29" spans="1:12" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_LOAD_01_001_CIBSE_LOAD</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+    </row>
+    <row r="30" spans="1:12" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_LOAD_02_001_ASHRAE_LOAD</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+    </row>
+    <row r="31" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>BP_ENE_01_001_IDEAL_SYSTEM</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H26:H27 H29:H30 H32 H19:H24 H15:H16 H8:H13 H3:H6">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="ALMOST">
+      <formula>NOT(ISERROR(SEARCH("ALMOST",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",H3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",H3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="ALMOST">
+      <formula>NOT(ISERROR(SEARCH("ALMOST",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",H5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="ALMOST">
+      <formula>NOT(ISERROR(SEARCH("ALMOST",H17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",H17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",H17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>